<commit_message>
Tabla dinámica con datos históricos
</commit_message>
<xml_diff>
--- a/02/TablaDinamica.xlsx
+++ b/02/TablaDinamica.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17835" windowHeight="8865"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17835" windowHeight="8865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TD-Poblacion" sheetId="7" r:id="rId1"/>
-    <sheet name="HistoricoMundial" sheetId="8" r:id="rId2"/>
-    <sheet name="Global" sheetId="1" r:id="rId3"/>
-    <sheet name="TD-PoblacionContinente" sheetId="5" r:id="rId4"/>
-    <sheet name="TD-SumaAreaTotal" sheetId="4" r:id="rId5"/>
-    <sheet name="InformeIdiomas" sheetId="6" r:id="rId6"/>
-    <sheet name="TD-IdiomaArea" sheetId="3" r:id="rId7"/>
-    <sheet name="TD-Idiomas" sheetId="2" r:id="rId8"/>
+    <sheet name="Hoja2" sheetId="10" r:id="rId2"/>
+    <sheet name="HistoricoMundial" sheetId="8" r:id="rId3"/>
+    <sheet name="Global" sheetId="1" r:id="rId4"/>
+    <sheet name="TD-PoblacionContinente" sheetId="5" r:id="rId5"/>
+    <sheet name="TD-SumaAreaTotal" sheetId="4" r:id="rId6"/>
+    <sheet name="InformeIdiomas" sheetId="6" r:id="rId7"/>
+    <sheet name="TD-IdiomaArea" sheetId="3" r:id="rId8"/>
+    <sheet name="TD-Idiomas" sheetId="2" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="SegmentaciónDeDatos_Continente">#N/A</definedName>
@@ -27,14 +28,15 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId9"/>
-    <pivotCache cacheId="22" r:id="rId10"/>
+    <pivotCache cacheId="0" r:id="rId10"/>
+    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="15" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
-        <x14:slicerCache r:id="rId11"/>
-        <x14:slicerCache r:id="rId12"/>
+        <x14:slicerCache r:id="rId13"/>
+        <x14:slicerCache r:id="rId14"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="274">
   <si>
     <t>Datos sobre población de 1.999, en miles de personas</t>
   </si>
@@ -847,6 +849,30 @@
   <si>
     <t>Población mundial</t>
   </si>
+  <si>
+    <t>Suma de Población mundial</t>
+  </si>
+  <si>
+    <t>1/1/1000</t>
+  </si>
+  <si>
+    <t>1/1/1650</t>
+  </si>
+  <si>
+    <t>1/1/1750</t>
+  </si>
+  <si>
+    <t>1/1/1800</t>
+  </si>
+  <si>
+    <t>1/1/1850</t>
+  </si>
+  <si>
+    <t>1/1/1900</t>
+  </si>
+  <si>
+    <t>1/1/1950</t>
+  </si>
 </sst>
 </file>
 
@@ -897,23 +923,23 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -922,8 +948,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -960,14 +986,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="NivelCol_1" xfId="2" builtinId="2" iLevel="0"/>
-    <cellStyle name="NivelCol_2" xfId="1" builtinId="2" iLevel="1"/>
+    <cellStyle name="NivelCol_1" xfId="1" builtinId="2" iLevel="0"/>
+    <cellStyle name="NivelCol_2" xfId="2" builtinId="2" iLevel="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1015,7 +1084,7 @@
         <c:idx val="4"/>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="10"/>
+        <c:idx val="5"/>
         <c:spPr>
           <a:gradFill rotWithShape="1">
             <a:gsLst>
@@ -1050,100 +1119,11 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="lt2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="5B9BD5">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF">
-                  <a:alpha val="50000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="11"/>
+        <c:idx val="6"/>
         <c:spPr>
           <a:gradFill rotWithShape="1">
             <a:gsLst>
@@ -1178,100 +1158,11 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="lt2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ED7D31">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF">
-                  <a:alpha val="50000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="12"/>
+        <c:idx val="7"/>
         <c:spPr>
           <a:gradFill rotWithShape="1">
             <a:gsLst>
@@ -1306,100 +1197,11 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="lt2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="A5A5A5">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF">
-                  <a:alpha val="50000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="13"/>
+        <c:idx val="8"/>
         <c:spPr>
           <a:gradFill rotWithShape="1">
             <a:gsLst>
@@ -1434,100 +1236,11 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="lt2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="FFC000">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF">
-                  <a:alpha val="50000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="14"/>
+        <c:idx val="9"/>
         <c:spPr>
           <a:gradFill rotWithShape="1">
             <a:gsLst>
@@ -1562,100 +1275,11 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent5">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent5">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:schemeClr val="lt2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472C4">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF">
-                  <a:alpha val="50000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="63500" dist="88900" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx2"/>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
       <c:pivotFmt>
-        <c:idx val="15"/>
+        <c:idx val="10"/>
         <c:spPr>
           <a:gradFill rotWithShape="1">
             <a:gsLst>
@@ -2430,6 +2054,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="484765160"/>
+        <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
         <a:noFill/>
@@ -3073,8 +2698,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Continente"/>
@@ -3091,7 +2716,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3145,8 +2770,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Idioma"/>
@@ -3163,7 +2788,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -3760,7 +3385,7 @@
     <cacheField name="% P. rural" numFmtId="10">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="1"/>
     </cacheField>
-    <cacheField name="Prevision 2010" numFmtId="0" formula="'Total país' * 1.08" databaseField="0"/>
+    <cacheField name="Prevision 2010" numFmtId="0" formula="'Total país'* 1.08" databaseField="0"/>
     <cacheField name="Total continente" numFmtId="0" formula="Rural+Urbana" databaseField="0"/>
   </cacheFields>
   <extLst>
@@ -3771,6 +3396,46 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Francisco Charte Ojeda" refreshedDate="42403.461222453705" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="18">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:B19" sheet="HistoricoMundial"/>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="Año" numFmtId="14">
+      <sharedItems containsDate="1" containsMixedTypes="1" minDate="1955-01-01T00:00:00" maxDate="2010-01-02T00:00:00" count="18">
+        <s v="1/1/1000"/>
+        <s v="1/1/1650"/>
+        <s v="1/1/1750"/>
+        <s v="1/1/1800"/>
+        <s v="1/1/1850"/>
+        <s v="1/1/1900"/>
+        <s v="1/1/1950"/>
+        <d v="1955-01-01T00:00:00"/>
+        <d v="1960-01-01T00:00:00"/>
+        <d v="1965-01-01T00:00:00"/>
+        <d v="1970-01-01T00:00:00"/>
+        <d v="1975-01-01T00:00:00"/>
+        <d v="1980-01-01T00:00:00"/>
+        <d v="1985-01-01T00:00:00"/>
+        <d v="1990-01-01T00:00:00"/>
+        <d v="1995-01-01T00:00:00"/>
+        <d v="2000-01-01T00:00:00"/>
+        <d v="2010-01-01T00:00:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Población mundial" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="410000" maxValue="6467978.5200000005"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="223">
   <r>
@@ -8687,8 +8352,85 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="18">
+  <r>
+    <x v="0"/>
+    <n v="410000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="545000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="791000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="981000"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="1262000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="1650000"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="2516000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2751000"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="3018000"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3335000"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="3697000"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="4077000"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="4446000"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="4854000"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="5259000"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="5759000"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="6228000"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <n v="6467978.5200000005"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica7" cacheId="22" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica7" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:G10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField axis="axisCol" showAll="0">
@@ -8782,7 +8524,7 @@
     <dataField name="Suma de Total continente" fld="10" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="6">
-    <chartFormat chart="0" format="10" series="1">
+    <chartFormat chart="0" format="5" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -8794,7 +8536,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="11" series="1">
+    <chartFormat chart="0" format="6" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -8806,7 +8548,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="12" series="1">
+    <chartFormat chart="0" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -8818,7 +8560,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="13" series="1">
+    <chartFormat chart="0" format="8" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -8830,7 +8572,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="14" series="1">
+    <chartFormat chart="0" format="9" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -8842,7 +8584,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="15" series="1">
+    <chartFormat chart="0" format="10" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -8862,7 +8604,131 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="22" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B22" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="19">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="19">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Población mundial" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica5" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField axis="axisRow" showAll="0">
@@ -8959,8 +8825,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -9275,8 +9141,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica6" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField axis="axisPage" showAll="0">
@@ -9603,8 +9469,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="9" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica2" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:J675" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisPage" showAll="0">
@@ -11932,8 +11798,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="9" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TablaDinámica1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:J21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -12382,8 +12248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12594,10 +12460,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A3:B22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" s="18">
+        <v>410000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>268</v>
+      </c>
+      <c r="B5" s="18">
+        <v>545000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="18">
+        <v>791000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="18">
+        <v>981000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="18">
+        <v>1262000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="18">
+        <v>1650000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="B10" s="18">
+        <v>2516000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="25">
+        <v>20090</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2751000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
+        <v>21916</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3018000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="25">
+        <v>23743</v>
+      </c>
+      <c r="B13" s="18">
+        <v>3335000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="25">
+        <v>25569</v>
+      </c>
+      <c r="B14" s="18">
+        <v>3697000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
+        <v>27395</v>
+      </c>
+      <c r="B15" s="18">
+        <v>4077000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="25">
+        <v>29221</v>
+      </c>
+      <c r="B16" s="18">
+        <v>4446000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
+        <v>31048</v>
+      </c>
+      <c r="B17" s="18">
+        <v>4854000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
+        <v>32874</v>
+      </c>
+      <c r="B18" s="18">
+        <v>5259000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
+        <v>34700</v>
+      </c>
+      <c r="B19" s="18">
+        <v>5759000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="25">
+        <v>36526</v>
+      </c>
+      <c r="B20" s="18">
+        <v>6228000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="25">
+        <v>40179</v>
+      </c>
+      <c r="B21" s="18">
+        <v>6467978.5200000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="18">
+        <v>58046978.520000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12605,7 +12650,7 @@
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>264</v>
       </c>
@@ -12613,157 +12658,175 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
-        <v>1000</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="26" t="s">
+        <v>267</v>
       </c>
       <c r="B2" s="22">
         <v>410000</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
-        <v>1650</v>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="s">
+        <v>268</v>
       </c>
       <c r="B3" s="22">
         <v>545000</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
-        <v>1750</v>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>269</v>
       </c>
       <c r="B4" s="22">
         <v>791000</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="21">
-        <v>1800</v>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>270</v>
       </c>
       <c r="B5" s="22">
         <v>981000</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
-        <v>1850</v>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
+        <v>271</v>
       </c>
       <c r="B6" s="23">
         <v>1262000</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
-        <v>1900</v>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>272</v>
       </c>
       <c r="B7" s="23">
         <v>1650000</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
-        <v>1950</v>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
+        <v>273</v>
       </c>
       <c r="B8" s="23">
         <v>2516000</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
-        <v>1955</v>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
+        <v>20090</v>
       </c>
       <c r="B9" s="23">
         <v>2751000</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
-        <v>1960</v>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
+        <v>21916</v>
       </c>
       <c r="B10" s="23">
         <v>3018000</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
-        <v>1965</v>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
+        <v>23743</v>
       </c>
       <c r="B11" s="23">
         <v>3335000</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
-        <v>1970</v>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
+        <v>25569</v>
       </c>
       <c r="B12" s="23">
         <v>3697000</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
-        <v>1975</v>
+      <c r="D12" s="21"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
+        <v>27395</v>
       </c>
       <c r="B13" s="23">
         <v>4077000</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
-        <v>1980</v>
+      <c r="D13" s="21"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
+        <v>29221</v>
       </c>
       <c r="B14" s="23">
         <v>4446000</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
-        <v>1985</v>
+      <c r="D14" s="21"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
+        <v>31048</v>
       </c>
       <c r="B15" s="23">
         <v>4854000</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
-        <v>1990</v>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
+        <v>32874</v>
       </c>
       <c r="B16" s="23">
         <v>5259000</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
-        <v>1995</v>
+      <c r="D16" s="21"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
+        <v>34700</v>
       </c>
       <c r="B17" s="23">
         <v>5759000</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
-        <v>2000</v>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
+        <v>36526</v>
       </c>
       <c r="B18" s="23">
         <v>6228000</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="24">
-        <v>2010</v>
+      <c r="D18" s="21"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <v>40179</v>
       </c>
       <c r="B19" s="14">
         <f>GETPIVOTDATA("Suma de Prevision 2010",'TD-Poblacion'!$A$3)</f>
         <v>6467978.5200000005</v>
       </c>
+      <c r="D19" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I233"/>
   <sheetViews>
@@ -19781,7 +19844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B20"/>
   <sheetViews>
@@ -19932,7 +19995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D12"/>
   <sheetViews>
@@ -20093,7 +20156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -20262,7 +20325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J675"/>
   <sheetViews>
@@ -31555,7 +31618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J21"/>
   <sheetViews>

</xml_diff>